<commit_message>
-Added 28 April Powerpoint presentation Bug fixes: Joe_plots.R -fixed the stress.resp.plot function so that it actually replicates the tbeta_rnd call. Joe_functions.R -commented out redundant and unnecessary code in the beta_param function.  The commented code can eventually be removed once we’re certain it wasn’t required.
</commit_message>
<xml_diff>
--- a/ARTR_Joe_model/stressor-response_fixed_ARTR.xlsx
+++ b/ARTR_Joe_model/stressor-response_fixed_ARTR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -14814,8 +14814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16025,8 +16025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16066,7 +16066,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -16080,10 +16080,10 @@
         <v>72.518552569214293</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -16097,13 +16097,13 @@
         <v>54.089744537631447</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E4">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -16114,13 +16114,13 @@
         <v>23.679425319502087</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -16137,7 +16137,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -16145,6 +16145,15 @@
         <v>31</v>
       </c>
       <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
         <v>0</v>
       </c>
     </row>
@@ -16584,7 +16593,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E20"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>